<commit_message>
Update JEE_FSD_Angular Mar 2nd Batch Project Groups.xlsx
</commit_message>
<xml_diff>
--- a/JEE_FSD_Angular Mar 2nd Batch Project Groups.xlsx
+++ b/JEE_FSD_Angular Mar 2nd Batch Project Groups.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\CorporateTraining\training 2021\20210305 CapGemnini Java EE Angular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubFolder\cgfsd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01699AD0-2F49-4EC1-9700-E5E174218264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DE96EB-CE7B-4AA8-ACB4-225AB4286521}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>Anurban Mahapatra</t>
   </si>
   <si>
-    <t>Ashish Veram</t>
-  </si>
-  <si>
     <t>Bommidi Surendra Babu</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>Md Inam</t>
   </si>
   <si>
-    <t>Sulabh Majumdar</t>
-  </si>
-  <si>
     <t>Surajit Mandal</t>
   </si>
   <si>
@@ -137,6 +131,12 @@
   </si>
   <si>
     <t>Teams</t>
+  </si>
+  <si>
+    <t>Ashish Verma</t>
+  </si>
+  <si>
+    <t>Sulabh Majumder</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -448,6 +448,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,8 +673,8 @@
   </sheetPr>
   <dimension ref="A1:X1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -712,7 +715,7 @@
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
@@ -792,11 +795,11 @@
     <row r="5" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -890,7 +893,7 @@
     <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="15"/>
@@ -1007,7 +1010,7 @@
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
@@ -1053,7 +1056,7 @@
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="15"/>
@@ -1076,7 +1079,7 @@
     <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="15"/>
@@ -1122,7 +1125,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>0</v>
@@ -1216,7 +1219,7 @@
     <row r="23" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15"/>
@@ -1285,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>0</v>
@@ -1310,7 +1313,7 @@
     <row r="27" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="13" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="15"/>
@@ -1356,7 +1359,7 @@
     <row r="29" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="15"/>
@@ -1448,7 +1451,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>0</v>
@@ -1496,7 +1499,7 @@
     <row r="35" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="15"/>
@@ -1570,7 +1573,7 @@
       <c r="X38" s="7"/>
     </row>
     <row r="39" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
+      <c r="A39" s="34">
         <v>6</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -1695,7 +1698,7 @@
     </row>
     <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="13" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="15"/>

</xml_diff>